<commit_message>
testing upload from my pc
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF13078-2F2E-48D7-A97C-50230616FACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D989C-AEDF-489B-B2AA-E363D828DC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="169">
   <si>
     <t>Play_VO_Alarm_Defective_Modules</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>asdasdasda</t>
+  </si>
+  <si>
+    <t>Tite ko malaki para kay rose</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
-  <dimension ref="A3:R967"/>
+  <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H222" sqref="H222"/>
+    <sheetView tabSelected="1" topLeftCell="A930" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F969" sqref="F969"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5995,6 +5998,11 @@
     <row r="967" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F967" s="1" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="968" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F968" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing upload from my pc (#23)
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF13078-2F2E-48D7-A97C-50230616FACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D989C-AEDF-489B-B2AA-E363D828DC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="169">
   <si>
     <t>Play_VO_Alarm_Defective_Modules</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>asdasdasda</t>
+  </si>
+  <si>
+    <t>Tite ko malaki para kay rose</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
-  <dimension ref="A3:R967"/>
+  <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H222" sqref="H222"/>
+    <sheetView tabSelected="1" topLeftCell="A930" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F969" sqref="F969"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5995,6 +5998,11 @@
     <row r="967" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F967" s="1" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="968" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F968" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VoDominationEvent and Excel File deployment update
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D989C-AEDF-489B-B2AA-E363D828DC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E016F-1F86-4F89-BF05-9A84E37F8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
+    <workbookView xWindow="90" yWindow="225" windowWidth="14250" windowHeight="7965" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="VO list" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="173">
   <si>
     <t>Play_VO_Alarm_Defective_Modules</t>
   </si>
@@ -544,6 +544,18 @@
   </si>
   <si>
     <t>Tite ko malaki para kay rose</t>
+  </si>
+  <si>
+    <t>VO_Domination_Advantage_Ally</t>
+  </si>
+  <si>
+    <t>VO_Domination_Advantage_Enemy</t>
+  </si>
+  <si>
+    <t>VO_Domination_Close_Win_Enemy</t>
+  </si>
+  <si>
+    <t>VO_Domination_Close_Win_Ally</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
   <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A930" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F969" sqref="F969"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H263" sqref="H263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,24 +2330,36 @@
         <v>38</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D243" s="1" t="s">
+    <row r="243" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D243" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D244" s="1" t="s">
+      <c r="F243" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D244" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D245" s="1" t="s">
+      <c r="F244" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D245" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D246" s="1" t="s">
+      <c r="F245" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D246" s="5" t="s">
         <v>89</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,23 +2372,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D249" s="1" t="s">
+    <row r="249" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D249" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D250" s="1" t="s">
+    <row r="250" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D250" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D251" s="1" t="s">
+    <row r="251" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D251" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D252" s="1" t="s">
+    <row r="252" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D252" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2373,23 +2397,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D254" s="1" t="s">
+    <row r="254" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D254" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D255" s="1" t="s">
+    <row r="255" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D255" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D256" s="1" t="s">
+    <row r="256" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D256" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D257" s="1" t="s">
+    <row r="257" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D257" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2398,23 +2422,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D259" s="1" t="s">
+    <row r="259" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D259" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D260" s="1" t="s">
+    <row r="260" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D260" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D261" s="1" t="s">
+    <row r="261" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D261" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D262" s="1" t="s">
+    <row r="262" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D262" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2423,23 +2447,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D264" s="1" t="s">
+    <row r="264" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D264" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D265" s="1" t="s">
+    <row r="265" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D265" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D266" s="1" t="s">
+    <row r="266" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D266" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D267" s="1" t="s">
+    <row r="267" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D267" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6438,7 +6462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BE8D90-371B-4FA4-BEF6-9B8645E31B40}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
VoDominationEvent and Excel File deployment update (#25)
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D989C-AEDF-489B-B2AA-E363D828DC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E016F-1F86-4F89-BF05-9A84E37F8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
+    <workbookView xWindow="90" yWindow="225" windowWidth="14250" windowHeight="7965" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="VO list" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="173">
   <si>
     <t>Play_VO_Alarm_Defective_Modules</t>
   </si>
@@ -544,6 +544,18 @@
   </si>
   <si>
     <t>Tite ko malaki para kay rose</t>
+  </si>
+  <si>
+    <t>VO_Domination_Advantage_Ally</t>
+  </si>
+  <si>
+    <t>VO_Domination_Advantage_Enemy</t>
+  </si>
+  <si>
+    <t>VO_Domination_Close_Win_Enemy</t>
+  </si>
+  <si>
+    <t>VO_Domination_Close_Win_Ally</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
   <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A930" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F969" sqref="F969"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H263" sqref="H263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,24 +2330,36 @@
         <v>38</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D243" s="1" t="s">
+    <row r="243" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D243" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D244" s="1" t="s">
+      <c r="F243" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D244" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D245" s="1" t="s">
+      <c r="F244" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D245" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D246" s="1" t="s">
+      <c r="F245" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D246" s="5" t="s">
         <v>89</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,23 +2372,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D249" s="1" t="s">
+    <row r="249" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D249" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D250" s="1" t="s">
+    <row r="250" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D250" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D251" s="1" t="s">
+    <row r="251" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D251" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D252" s="1" t="s">
+    <row r="252" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D252" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2373,23 +2397,23 @@
         <v>41</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D254" s="1" t="s">
+    <row r="254" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D254" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D255" s="1" t="s">
+    <row r="255" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D255" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D256" s="1" t="s">
+    <row r="256" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D256" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D257" s="1" t="s">
+    <row r="257" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D257" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2398,23 +2422,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D259" s="1" t="s">
+    <row r="259" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D259" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D260" s="1" t="s">
+    <row r="260" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D260" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D261" s="1" t="s">
+    <row r="261" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D261" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D262" s="1" t="s">
+    <row r="262" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D262" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2423,23 +2447,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D264" s="1" t="s">
+    <row r="264" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D264" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D265" s="1" t="s">
+    <row r="265" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D265" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D266" s="1" t="s">
+    <row r="266" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D266" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D267" s="1" t="s">
+    <row r="267" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D267" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6438,7 +6462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BE8D90-371B-4FA4-BEF6-9B8645E31B40}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Manual Coding for Vo FireAlarm submit double kill and update xls
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E016F-1F86-4F89-BF05-9A84E37F8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0F4442-0336-4F75-A67B-77E0395BE46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="225" windowWidth="14250" windowHeight="7965" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
+    <workbookView xWindow="14400" yWindow="7125" windowWidth="14400" windowHeight="8625" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="VO list" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +608,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -621,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -636,6 +642,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
   <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H263" sqref="H263"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,33 +2482,33 @@
         <v>165</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B269" s="1" t="s">
+    <row r="269" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B269" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B270" s="1" t="s">
+    <row r="270" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B270" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C271" s="1" t="s">
+    <row r="271" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C271" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C272" s="1" t="s">
+    <row r="272" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C272" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C273" s="1" t="s">
+    <row r="273" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C273" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C274" s="1" t="s">
+    <row r="274" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C274" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2518,8 +2525,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D277" s="1" t="s">
+    <row r="277" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D277" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2528,43 +2535,43 @@
         <v>39</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C279" s="1" t="s">
+    <row r="279" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C279" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D280" s="1" t="s">
+    <row r="280" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D280" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C281" s="1" t="s">
+    <row r="281" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C281" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D282" s="1" t="s">
+    <row r="282" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D282" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C283" s="1" t="s">
+    <row r="283" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C283" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D284" s="1" t="s">
+    <row r="284" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D284" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C285" s="1" t="s">
+    <row r="285" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C285" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D286" s="1" t="s">
+    <row r="286" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D286" s="8" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manual Coding for Vo FireAlarm submit double kill and update xls (#26)
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E016F-1F86-4F89-BF05-9A84E37F8AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0F4442-0336-4F75-A67B-77E0395BE46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="225" windowWidth="14250" windowHeight="7965" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
+    <workbookView xWindow="14400" yWindow="7125" windowWidth="14400" windowHeight="8625" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="VO list" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +608,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -621,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -636,6 +642,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
   <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H263" sqref="H263"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,33 +2482,33 @@
         <v>165</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B269" s="1" t="s">
+    <row r="269" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B269" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B270" s="1" t="s">
+    <row r="270" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B270" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C271" s="1" t="s">
+    <row r="271" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C271" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C272" s="1" t="s">
+    <row r="272" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C272" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C273" s="1" t="s">
+    <row r="273" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C273" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C274" s="1" t="s">
+    <row r="274" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C274" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2518,8 +2525,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D277" s="1" t="s">
+    <row r="277" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D277" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2528,43 +2535,43 @@
         <v>39</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C279" s="1" t="s">
+    <row r="279" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C279" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D280" s="1" t="s">
+    <row r="280" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D280" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C281" s="1" t="s">
+    <row r="281" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C281" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D282" s="1" t="s">
+    <row r="282" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D282" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C283" s="1" t="s">
+    <row r="283" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C283" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D284" s="1" t="s">
+    <row r="284" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D284" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C285" s="1" t="s">
+    <row r="285" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C285" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D286" s="1" t="s">
+    <row r="286" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D286" s="8" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove redundant file (#27)
</commit_message>
<xml_diff>
--- a/Haifuri Mod VO Spreadsheet.xlsx
+++ b/Haifuri Mod VO Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nightstalkers\Documents\GitHub Projects\Wows_Haifuri_VoiceMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0F4442-0336-4F75-A67B-77E0395BE46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558B5FA5-97AE-48E3-9A8B-8F68111B7DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="7125" windowWidth="14400" windowHeight="8625" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
+    <workbookView xWindow="12885" yWindow="2175" windowWidth="14250" windowHeight="7965" xr2:uid="{5CFBD424-2FA9-4BA6-BF78-1A890E70EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="VO list" sheetId="1" r:id="rId1"/>
@@ -1084,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759EC224-9B23-4D49-A9A9-4E8008F27D18}">
   <dimension ref="A3:R968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C285" sqref="C285"/>
+    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A332" sqref="A332:XFD337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2583,33 +2583,33 @@
         <v>165</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B288" s="1" t="s">
+    <row r="288" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B288" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B289" s="1" t="s">
+    <row r="289" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B289" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C290" s="1" t="s">
+    <row r="290" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C290" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C291" s="1" t="s">
+    <row r="291" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C291" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C292" s="1" t="s">
+    <row r="292" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C292" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C293" s="1" t="s">
+    <row r="293" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C293" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2621,183 +2621,183 @@
         <v>165</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B295" s="1" t="s">
+    <row r="295" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B295" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D296" s="1" t="s">
+    <row r="296" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D296" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E297" s="1" t="s">
+    <row r="297" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E297" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E298" s="1" t="s">
+    <row r="298" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E298" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E299" s="1" t="s">
+    <row r="299" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E299" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E300" s="1" t="s">
+    <row r="300" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E300" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E301" s="1" t="s">
+    <row r="301" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E301" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B302" s="1" t="s">
+    <row r="302" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B302" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C303" s="1" t="s">
+    <row r="303" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C303" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D304" s="1" t="s">
+    <row r="304" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D304" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="305" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E305" s="1" t="s">
+    <row r="305" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E305" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="306" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E306" s="1" t="s">
+    <row r="306" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E306" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="307" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E307" s="1" t="s">
+    <row r="307" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E307" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="308" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E308" s="1" t="s">
+    <row r="308" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E308" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="309" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E309" s="1" t="s">
+    <row r="309" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E309" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="310" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C310" s="1" t="s">
+    <row r="310" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C310" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="311" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D311" s="1" t="s">
+    <row r="311" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D311" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="312" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E312" s="1" t="s">
+    <row r="312" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E312" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="313" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E313" s="1" t="s">
+    <row r="313" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E313" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="314" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E314" s="1" t="s">
+    <row r="314" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E314" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="315" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E315" s="1" t="s">
+    <row r="315" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E315" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="316" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E316" s="1" t="s">
+    <row r="316" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E316" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="317" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C317" s="1" t="s">
+    <row r="317" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C317" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="318" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D318" s="1" t="s">
+    <row r="318" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D318" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="319" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E319" s="1" t="s">
+    <row r="319" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E319" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="320" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E320" s="1" t="s">
+    <row r="320" spans="3:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E320" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E321" s="1" t="s">
+    <row r="321" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E321" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E322" s="1" t="s">
+    <row r="322" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E322" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E323" s="1" t="s">
+    <row r="323" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E323" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C324" s="1" t="s">
+    <row r="324" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C324" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D325" s="1" t="s">
+    <row r="325" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D325" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E326" s="1" t="s">
+    <row r="326" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E326" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E327" s="1" t="s">
+    <row r="327" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E327" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E328" s="1" t="s">
+    <row r="328" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E328" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E329" s="1" t="s">
+    <row r="329" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E329" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E330" s="1" t="s">
+    <row r="330" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E330" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2809,33 +2809,33 @@
         <v>165</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B332" s="1" t="s">
+    <row r="332" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B332" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B333" s="1" t="s">
+    <row r="333" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B333" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C334" s="1" t="s">
+    <row r="334" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C334" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C335" s="1" t="s">
+    <row r="335" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C335" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C336" s="1" t="s">
+    <row r="336" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C336" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C337" s="1" t="s">
+    <row r="337" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C337" s="5" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>